<commit_message>
Added all code together and made graphs output to folder
</commit_message>
<xml_diff>
--- a/Resources/totalmoviedf.xlsx
+++ b/Resources/totalmoviedf.xlsx
@@ -620,7 +620,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>1,172,062</t>
+          <t>1,180,832</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>1,338,789</t>
+          <t>1,342,345</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -950,7 +950,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>655,241</t>
+          <t>657,123</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1,411,647</t>
+          <t>1,416,271</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -1214,7 +1214,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2,707,874</t>
+          <t>2,719,396</t>
         </is>
       </c>
       <c r="M12" t="n">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>821,772</t>
+          <t>825,050</t>
         </is>
       </c>
       <c r="M16" t="n">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>479,363</t>
+          <t>481,363</t>
         </is>
       </c>
       <c r="M20" t="n">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>576,344</t>
+          <t>579,690</t>
         </is>
       </c>
       <c r="M22" t="n">
@@ -2204,7 +2204,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>852,161</t>
+          <t>855,253</t>
         </is>
       </c>
       <c r="M27" t="n">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>672,323</t>
+          <t>674,701</t>
         </is>
       </c>
       <c r="M28" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>866,350</t>
+          <t>869,524</t>
         </is>
       </c>
       <c r="M29" t="n">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>944,016</t>
+          <t>948,650</t>
         </is>
       </c>
       <c r="M31" t="n">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>260,486</t>
+          <t>262,152</t>
         </is>
       </c>
       <c r="M32" t="n">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>394,798</t>
+          <t>397,057</t>
         </is>
       </c>
       <c r="M33" t="n">
@@ -2732,7 +2732,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>835,243</t>
+          <t>838,781</t>
         </is>
       </c>
       <c r="M35" t="n">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>637,653</t>
+          <t>639,630</t>
         </is>
       </c>
       <c r="M38" t="n">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>897,089</t>
+          <t>900,765</t>
         </is>
       </c>
       <c r="M40" t="n">
@@ -3128,7 +3128,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>1,063,048</t>
+          <t>1,066,868</t>
         </is>
       </c>
       <c r="M41" t="n">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>808,693</t>
+          <t>812,204</t>
         </is>
       </c>
       <c r="M42" t="n">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>1,880,828</t>
+          <t>1,887,528</t>
         </is>
       </c>
       <c r="M43" t="n">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>207,856</t>
+          <t>208,563</t>
         </is>
       </c>
       <c r="M46" t="n">
@@ -3590,7 +3590,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>282,639</t>
+          <t>283,674</t>
         </is>
       </c>
       <c r="M48" t="n">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>1,063,020</t>
+          <t>1,068,226</t>
         </is>
       </c>
       <c r="M49" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>512,109</t>
+          <t>516,213</t>
         </is>
       </c>
       <c r="M51" t="n">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>397,653</t>
+          <t>400,739</t>
         </is>
       </c>
       <c r="M52" t="n">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>514,126</t>
+          <t>516,590</t>
         </is>
       </c>
       <c r="M57" t="n">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>605,236</t>
+          <t>607,943</t>
         </is>
       </c>
       <c r="M59" t="n">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>488,854</t>
+          <t>491,465</t>
         </is>
       </c>
       <c r="M61" t="n">
@@ -4514,7 +4514,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>676,321</t>
+          <t>680,531</t>
         </is>
       </c>
       <c r="M62" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>1,202,800</t>
+          <t>1,218,697</t>
         </is>
       </c>
       <c r="M64" t="n">
@@ -4976,7 +4976,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>601,772</t>
+          <t>605,526</t>
         </is>
       </c>
       <c r="M69" t="n">
@@ -5174,7 +5174,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>1,078,398</t>
+          <t>1,082,676</t>
         </is>
       </c>
       <c r="M72" t="n">
@@ -5240,7 +5240,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>806,183</t>
+          <t>809,596</t>
         </is>
       </c>
       <c r="M73" t="n">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>463,938</t>
+          <t>465,456</t>
         </is>
       </c>
       <c r="M74" t="n">
@@ -5372,7 +5372,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>1,909,902</t>
+          <t>1,916,428</t>
         </is>
       </c>
       <c r="M75" t="n">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>771,884</t>
+          <t>776,377</t>
         </is>
       </c>
       <c r="M76" t="n">
@@ -5570,7 +5570,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>726,652</t>
+          <t>729,711</t>
         </is>
       </c>
       <c r="M78" t="n">
@@ -5966,7 +5966,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>842,144</t>
+          <t>844,125</t>
         </is>
       </c>
       <c r="M84" t="n">
@@ -6164,7 +6164,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>290,082</t>
+          <t>290,764</t>
         </is>
       </c>
       <c r="M87" t="n">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>565,728</t>
+          <t>568,103</t>
         </is>
       </c>
       <c r="M88" t="n">
@@ -6428,7 +6428,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>2,403,698</t>
+          <t>2,414,022</t>
         </is>
       </c>
       <c r="M91" t="n">
@@ -6740,7 +6740,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>20 Jun 1980</t>
+          <t>18 Jun 1980</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -6758,7 +6758,7 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>1,316,200</t>
+          <t>1,321,413</t>
         </is>
       </c>
       <c r="M96" t="n">
@@ -6824,7 +6824,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>644,503</t>
+          <t>647,099</t>
         </is>
       </c>
       <c r="M97" t="n">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>606,961</t>
+          <t>608,778</t>
         </is>
       </c>
       <c r="M101" t="n">
@@ -7154,7 +7154,7 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>245,690</t>
+          <t>246,266</t>
         </is>
       </c>
       <c r="M102" t="n">
@@ -7286,7 +7286,7 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>804,845</t>
+          <t>808,123</t>
         </is>
       </c>
       <c r="M104" t="n">
@@ -7352,7 +7352,7 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>839,057</t>
+          <t>840,905</t>
         </is>
       </c>
       <c r="M105" t="n">
@@ -7614,7 +7614,7 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>697,228</t>
+          <t>700,046</t>
         </is>
       </c>
       <c r="M109" t="n">
@@ -7746,7 +7746,7 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>654,001</t>
+          <t>656,767</t>
         </is>
       </c>
       <c r="M111" t="n">
@@ -7812,7 +7812,7 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>670,012</t>
+          <t>672,781</t>
         </is>
       </c>
       <c r="M112" t="n">
@@ -8010,7 +8010,7 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>621,232</t>
+          <t>624,212</t>
         </is>
       </c>
       <c r="M115" t="n">
@@ -8076,7 +8076,7 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>862,976</t>
+          <t>866,915</t>
         </is>
       </c>
       <c r="M116" t="n">
@@ -8472,7 +8472,7 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>546,113</t>
+          <t>547,863</t>
         </is>
       </c>
       <c r="M122" t="n">
@@ -8670,7 +8670,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>385,938</t>
+          <t>387,430</t>
         </is>
       </c>
       <c r="M125" t="n">
@@ -8736,7 +8736,7 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>359,324</t>
+          <t>360,720</t>
         </is>
       </c>
       <c r="M126" t="n">
@@ -8868,7 +8868,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>653,059</t>
+          <t>655,775</t>
         </is>
       </c>
       <c r="M128" t="n">
@@ -8957,7 +8957,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Raiders of the Lost Ark</t>
+          <t>Indiana Jones and the Raiders of the Lost Ark</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -9000,7 +9000,7 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>983,111</t>
+          <t>986,622</t>
         </is>
       </c>
       <c r="M130" t="n">
@@ -9528,7 +9528,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>384,957</t>
+          <t>386,272</t>
         </is>
       </c>
       <c r="M138" t="n">
@@ -9594,7 +9594,7 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>539,786</t>
+          <t>541,647</t>
         </is>
       </c>
       <c r="M139" t="n">
@@ -9726,7 +9726,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>401,575</t>
+          <t>404,246</t>
         </is>
       </c>
       <c r="M141" t="n">
@@ -10518,7 +10518,7 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>461,729</t>
+          <t>463,164</t>
         </is>
       </c>
       <c r="M153" t="n">
@@ -11178,7 +11178,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>474,465</t>
+          <t>476,742</t>
         </is>
       </c>
       <c r="M163" t="n">
@@ -11244,7 +11244,7 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>343,365</t>
+          <t>345,133</t>
         </is>
       </c>
       <c r="M164" t="n">
@@ -11640,7 +11640,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>432,238</t>
+          <t>433,386</t>
         </is>
       </c>
       <c r="M170" t="n">
@@ -12036,7 +12036,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>1,418,536</t>
+          <t>1,423,690</t>
         </is>
       </c>
       <c r="M176" t="n">
@@ -12564,7 +12564,7 @@
       </c>
       <c r="L184" t="inlineStr">
         <is>
-          <t>358,873</t>
+          <t>361,009</t>
         </is>
       </c>
       <c r="M184" t="n">
@@ -12630,7 +12630,7 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>502,394</t>
+          <t>505,849</t>
         </is>
       </c>
       <c r="M185" t="n">
@@ -12762,7 +12762,7 @@
       </c>
       <c r="L187" t="inlineStr">
         <is>
-          <t>834,525</t>
+          <t>836,719</t>
         </is>
       </c>
       <c r="M187" t="n">
@@ -12828,7 +12828,7 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>1,233,438</t>
+          <t>1,239,275</t>
         </is>
       </c>
       <c r="M188" t="n">
@@ -12960,7 +12960,7 @@
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>530,179</t>
+          <t>534,345</t>
         </is>
       </c>
       <c r="M190" t="n">
@@ -13422,7 +13422,7 @@
       </c>
       <c r="L197" t="inlineStr">
         <is>
-          <t>762,233</t>
+          <t>766,831</t>
         </is>
       </c>
       <c r="M197" t="n">
@@ -13620,7 +13620,7 @@
       </c>
       <c r="L200" t="inlineStr">
         <is>
-          <t>1,119,363</t>
+          <t>1,123,279</t>
         </is>
       </c>
       <c r="M200" t="n">
@@ -13686,7 +13686,7 @@
       </c>
       <c r="L201" t="inlineStr">
         <is>
-          <t>510,622</t>
+          <t>512,852</t>
         </is>
       </c>
       <c r="M201" t="n">
@@ -14016,7 +14016,7 @@
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>168,755</t>
+          <t>169,993</t>
         </is>
       </c>
       <c r="M206" t="n">
@@ -14346,7 +14346,7 @@
       </c>
       <c r="L211" t="inlineStr">
         <is>
-          <t>449,805</t>
+          <t>451,032</t>
         </is>
       </c>
       <c r="M211" t="n">
@@ -14544,7 +14544,7 @@
       </c>
       <c r="L214" t="inlineStr">
         <is>
-          <t>768,797</t>
+          <t>771,485</t>
         </is>
       </c>
       <c r="M214" t="n">
@@ -14940,7 +14940,7 @@
       </c>
       <c r="L220" t="inlineStr">
         <is>
-          <t>1,014,355</t>
+          <t>1,018,595</t>
         </is>
       </c>
       <c r="M220" t="n">
@@ -15596,11 +15596,11 @@
         </is>
       </c>
       <c r="K230" t="n">
-        <v>8.6</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>1,898,118</t>
+          <t>1,911,244</t>
         </is>
       </c>
       <c r="M230" t="n">
@@ -15666,7 +15666,7 @@
       </c>
       <c r="L231" t="inlineStr">
         <is>
-          <t>1,530,546</t>
+          <t>1,536,726</t>
         </is>
       </c>
       <c r="M231" t="n">
@@ -16854,7 +16854,7 @@
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>329,583</t>
+          <t>330,405</t>
         </is>
       </c>
       <c r="M249" t="n">
@@ -16920,7 +16920,7 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>865,173</t>
+          <t>869,015</t>
         </is>
       </c>
       <c r="M250" t="n">
@@ -17052,7 +17052,7 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>689,231</t>
+          <t>693,281</t>
         </is>
       </c>
       <c r="M252" t="n">
@@ -17974,7 +17974,7 @@
       </c>
       <c r="L266" t="inlineStr">
         <is>
-          <t>861,357</t>
+          <t>864,860</t>
         </is>
       </c>
       <c r="M266" t="n">
@@ -18370,7 +18370,7 @@
       </c>
       <c r="L272" t="inlineStr">
         <is>
-          <t>158,600</t>
+          <t>160,064</t>
         </is>
       </c>
       <c r="M272" t="n">
@@ -18502,7 +18502,7 @@
       </c>
       <c r="L274" t="inlineStr">
         <is>
-          <t>132,509</t>
+          <t>133,253</t>
         </is>
       </c>
       <c r="M274" t="n">
@@ -19294,7 +19294,7 @@
       </c>
       <c r="L286" t="inlineStr">
         <is>
-          <t>90,994</t>
+          <t>91,415</t>
         </is>
       </c>
       <c r="M286" t="n">
@@ -20152,7 +20152,7 @@
       </c>
       <c r="L299" t="inlineStr">
         <is>
-          <t>328,622</t>
+          <t>330,072</t>
         </is>
       </c>
       <c r="M299" t="n">
@@ -21010,7 +21010,7 @@
       </c>
       <c r="L312" t="inlineStr">
         <is>
-          <t>528,592</t>
+          <t>531,017</t>
         </is>
       </c>
       <c r="M312" t="n">
@@ -21274,7 +21274,7 @@
       </c>
       <c r="L316" t="inlineStr">
         <is>
-          <t>312,752</t>
+          <t>313,851</t>
         </is>
       </c>
       <c r="M316" t="n">
@@ -21340,7 +21340,7 @@
       </c>
       <c r="L317" t="inlineStr">
         <is>
-          <t>1,592,776</t>
+          <t>1,600,051</t>
         </is>
       </c>
       <c r="M317" t="n">
@@ -22066,7 +22066,7 @@
       </c>
       <c r="L328" t="inlineStr">
         <is>
-          <t>292,527</t>
+          <t>293,783</t>
         </is>
       </c>
       <c r="M328" t="n">
@@ -23384,7 +23384,7 @@
       </c>
       <c r="L348" t="inlineStr">
         <is>
-          <t>1,026,101</t>
+          <t>1,030,594</t>
         </is>
       </c>
       <c r="M348" t="n">
@@ -23582,7 +23582,7 @@
       </c>
       <c r="L351" t="inlineStr">
         <is>
-          <t>124,032</t>
+          <t>124,525</t>
         </is>
       </c>
       <c r="M351" t="n">
@@ -23714,7 +23714,7 @@
       </c>
       <c r="L353" t="inlineStr">
         <is>
-          <t>233,330</t>
+          <t>234,168</t>
         </is>
       </c>
       <c r="M353" t="n">
@@ -23780,7 +23780,7 @@
       </c>
       <c r="L354" t="inlineStr">
         <is>
-          <t>107,630</t>
+          <t>108,719</t>
         </is>
       </c>
       <c r="M354" t="n">
@@ -25296,7 +25296,7 @@
       </c>
       <c r="L377" t="inlineStr">
         <is>
-          <t>113,275</t>
+          <t>113,606</t>
         </is>
       </c>
       <c r="M377" t="n">
@@ -25758,7 +25758,7 @@
       </c>
       <c r="L384" t="inlineStr">
         <is>
-          <t>563,373</t>
+          <t>565,776</t>
         </is>
       </c>
       <c r="M384" t="n">
@@ -26612,7 +26612,7 @@
       </c>
       <c r="L397" t="inlineStr">
         <is>
-          <t>282,639</t>
+          <t>283,674</t>
         </is>
       </c>
       <c r="M397" t="n">
@@ -28128,7 +28128,7 @@
       </c>
       <c r="L420" t="inlineStr">
         <is>
-          <t>998,961</t>
+          <t>1,004,114</t>
         </is>
       </c>
       <c r="M420" t="n">
@@ -29250,7 +29250,7 @@
       </c>
       <c r="L437" t="inlineStr">
         <is>
-          <t>1,901,273</t>
+          <t>1,910,007</t>
         </is>
       </c>
       <c r="M437" t="n">
@@ -29646,7 +29646,7 @@
       </c>
       <c r="L443" t="inlineStr">
         <is>
-          <t>179,943</t>
+          <t>180,691</t>
         </is>
       </c>
       <c r="M443" t="n">
@@ -30570,7 +30570,7 @@
       </c>
       <c r="L457" t="inlineStr">
         <is>
-          <t>270,573</t>
+          <t>271,189</t>
         </is>
       </c>
       <c r="M457" t="n">
@@ -30768,7 +30768,7 @@
       </c>
       <c r="L460" t="inlineStr">
         <is>
-          <t>213,352</t>
+          <t>213,809</t>
         </is>
       </c>
       <c r="M460" t="n">
@@ -31164,7 +31164,7 @@
       </c>
       <c r="L466" t="inlineStr">
         <is>
-          <t>244,564</t>
+          <t>245,374</t>
         </is>
       </c>
       <c r="M466" t="n">
@@ -31296,7 +31296,7 @@
       </c>
       <c r="L468" t="inlineStr">
         <is>
-          <t>157,207</t>
+          <t>158,213</t>
         </is>
       </c>
       <c r="M468" t="n">
@@ -31758,7 +31758,7 @@
       </c>
       <c r="L475" t="inlineStr">
         <is>
-          <t>683,408</t>
+          <t>686,779</t>
         </is>
       </c>
       <c r="M475" t="n">
@@ -32814,7 +32814,7 @@
       </c>
       <c r="L491" t="inlineStr">
         <is>
-          <t>360,031</t>
+          <t>360,910</t>
         </is>
       </c>
       <c r="M491" t="n">
@@ -33144,7 +33144,7 @@
       </c>
       <c r="L496" t="inlineStr">
         <is>
-          <t>180,922</t>
+          <t>181,388</t>
         </is>
       </c>
       <c r="M496" t="n">
@@ -33474,7 +33474,7 @@
       </c>
       <c r="L501" t="inlineStr">
         <is>
-          <t>1,112,169</t>
+          <t>1,117,629</t>
         </is>
       </c>
       <c r="M501" t="n">
@@ -34332,7 +34332,7 @@
       </c>
       <c r="L514" t="inlineStr">
         <is>
-          <t>433,495</t>
+          <t>435,545</t>
         </is>
       </c>
       <c r="M514" t="n">
@@ -35648,7 +35648,7 @@
       </c>
       <c r="L534" t="inlineStr">
         <is>
-          <t>1,485,476</t>
+          <t>1,492,402</t>
         </is>
       </c>
       <c r="M534" t="n">
@@ -36506,7 +36506,7 @@
       </c>
       <c r="L547" t="inlineStr">
         <is>
-          <t>130,721</t>
+          <t>130,842</t>
         </is>
       </c>
       <c r="M547" t="n">
@@ -36572,7 +36572,7 @@
       </c>
       <c r="L548" t="inlineStr">
         <is>
-          <t>119,972</t>
+          <t>120,312</t>
         </is>
       </c>
       <c r="M548" t="n">
@@ -37232,7 +37232,7 @@
       </c>
       <c r="L558" t="inlineStr">
         <is>
-          <t>147,041</t>
+          <t>147,894</t>
         </is>
       </c>
       <c r="M558" t="n">
@@ -37430,7 +37430,7 @@
       </c>
       <c r="L561" t="inlineStr">
         <is>
-          <t>150,589</t>
+          <t>150,914</t>
         </is>
       </c>
       <c r="M561" t="n">
@@ -37496,7 +37496,7 @@
       </c>
       <c r="L562" t="inlineStr">
         <is>
-          <t>1,455,295</t>
+          <t>1,463,606</t>
         </is>
       </c>
       <c r="M562" t="n">
@@ -37628,7 +37628,7 @@
       </c>
       <c r="L564" t="inlineStr">
         <is>
-          <t>90,247</t>
+          <t>90,626</t>
         </is>
       </c>
       <c r="M564" t="n">
@@ -38156,7 +38156,7 @@
       </c>
       <c r="L572" t="inlineStr">
         <is>
-          <t>693,246</t>
+          <t>695,094</t>
         </is>
       </c>
       <c r="M572" t="n">
@@ -39608,7 +39608,7 @@
       </c>
       <c r="L594" t="inlineStr">
         <is>
-          <t>95,084</t>
+          <t>95,346</t>
         </is>
       </c>
       <c r="M594" t="n">
@@ -39938,7 +39938,7 @@
       </c>
       <c r="L599" t="inlineStr">
         <is>
-          <t>130,394</t>
+          <t>130,880</t>
         </is>
       </c>
       <c r="M599" t="n">
@@ -40532,7 +40532,7 @@
       </c>
       <c r="L608" t="inlineStr">
         <is>
-          <t>427,970</t>
+          <t>429,334</t>
         </is>
       </c>
       <c r="M608" t="n">
@@ -41786,7 +41786,7 @@
       </c>
       <c r="L627" t="inlineStr">
         <is>
-          <t>58,731</t>
+          <t>59,012</t>
         </is>
       </c>
       <c r="M627" t="n">
@@ -42050,7 +42050,7 @@
       </c>
       <c r="L631" t="inlineStr">
         <is>
-          <t>2,101,116</t>
+          <t>2,110,312</t>
         </is>
       </c>
       <c r="M631" t="n">
@@ -42182,7 +42182,7 @@
       </c>
       <c r="L633" t="inlineStr">
         <is>
-          <t>563,242</t>
+          <t>567,058</t>
         </is>
       </c>
       <c r="M633" t="n">
@@ -42380,7 +42380,7 @@
       </c>
       <c r="L636" t="inlineStr">
         <is>
-          <t>561,595</t>
+          <t>562,910</t>
         </is>
       </c>
       <c r="M636" t="n">
@@ -43434,7 +43434,7 @@
       </c>
       <c r="L652" t="inlineStr">
         <is>
-          <t>51,289</t>
+          <t>51,492</t>
         </is>
       </c>
       <c r="M652" t="n">
@@ -43896,7 +43896,7 @@
       </c>
       <c r="L659" t="inlineStr">
         <is>
-          <t>275,183</t>
+          <t>275,948</t>
         </is>
       </c>
       <c r="M659" t="n">
@@ -44886,7 +44886,7 @@
       </c>
       <c r="L674" t="inlineStr">
         <is>
-          <t>252,447</t>
+          <t>253,426</t>
         </is>
       </c>
       <c r="M674" t="n">
@@ -46074,7 +46074,7 @@
       </c>
       <c r="L692" t="inlineStr">
         <is>
-          <t>285,024</t>
+          <t>285,959</t>
         </is>
       </c>
       <c r="M692" t="n">
@@ -47460,7 +47460,7 @@
       </c>
       <c r="L713" t="inlineStr">
         <is>
-          <t>715,635</t>
+          <t>719,298</t>
         </is>
       </c>
       <c r="M713" t="n">
@@ -47782,7 +47782,7 @@
       </c>
       <c r="J718" t="inlineStr">
         <is>
-          <t>Adventure, Family, Fantasy</t>
+          <t>Adventure, Drama, Family</t>
         </is>
       </c>
       <c r="K718" t="n">
@@ -47790,7 +47790,7 @@
       </c>
       <c r="L718" t="inlineStr">
         <is>
-          <t>46,227</t>
+          <t>46,423</t>
         </is>
       </c>
       <c r="M718" t="n">
@@ -48648,7 +48648,7 @@
       </c>
       <c r="L731" t="inlineStr">
         <is>
-          <t>351,789</t>
+          <t>352,938</t>
         </is>
       </c>
       <c r="M731" t="n">
@@ -48912,7 +48912,7 @@
       </c>
       <c r="L735" t="inlineStr">
         <is>
-          <t>395,179</t>
+          <t>396,022</t>
         </is>
       </c>
       <c r="M735" t="n">
@@ -49704,7 +49704,7 @@
       </c>
       <c r="L747" t="inlineStr">
         <is>
-          <t>1,380,424</t>
+          <t>1,385,429</t>
         </is>
       </c>
       <c r="M747" t="n">
@@ -50034,7 +50034,7 @@
       </c>
       <c r="L752" t="inlineStr">
         <is>
-          <t>308,218</t>
+          <t>309,301</t>
         </is>
       </c>
       <c r="M752" t="n">
@@ -50760,7 +50760,7 @@
       </c>
       <c r="L763" t="inlineStr">
         <is>
-          <t>133,142</t>
+          <t>133,352</t>
         </is>
       </c>
       <c r="M763" t="n">
@@ -51750,7 +51750,7 @@
       </c>
       <c r="L778" t="inlineStr">
         <is>
-          <t>60,919</t>
+          <t>61,049</t>
         </is>
       </c>
       <c r="M778" t="n">
@@ -52476,7 +52476,7 @@
       </c>
       <c r="L789" t="inlineStr">
         <is>
-          <t>599,573</t>
+          <t>604,224</t>
         </is>
       </c>
       <c r="M789" t="n">
@@ -52542,7 +52542,7 @@
       </c>
       <c r="L790" t="inlineStr">
         <is>
-          <t>128,434</t>
+          <t>128,833</t>
         </is>
       </c>
       <c r="M790" t="n">
@@ -52608,7 +52608,7 @@
       </c>
       <c r="L791" t="inlineStr">
         <is>
-          <t>48,797</t>
+          <t>48,923</t>
         </is>
       </c>
       <c r="M791" t="n">
@@ -53202,7 +53202,7 @@
       </c>
       <c r="L800" t="inlineStr">
         <is>
-          <t>786,752</t>
+          <t>789,236</t>
         </is>
       </c>
       <c r="M800" t="n">
@@ -54192,7 +54192,7 @@
       </c>
       <c r="L815" t="inlineStr">
         <is>
-          <t>283,726</t>
+          <t>284,512</t>
         </is>
       </c>
       <c r="M815" t="n">
@@ -54852,7 +54852,7 @@
       </c>
       <c r="L825" t="inlineStr">
         <is>
-          <t>193,443</t>
+          <t>193,931</t>
         </is>
       </c>
       <c r="M825" t="n">
@@ -54918,7 +54918,7 @@
       </c>
       <c r="L826" t="inlineStr">
         <is>
-          <t>82,877</t>
+          <t>83,106</t>
         </is>
       </c>
       <c r="M826" t="n">
@@ -56238,7 +56238,7 @@
       </c>
       <c r="L846" t="inlineStr">
         <is>
-          <t>303,592</t>
+          <t>305,460</t>
         </is>
       </c>
       <c r="M846" t="n">
@@ -56502,7 +56502,7 @@
       </c>
       <c r="L850" t="inlineStr">
         <is>
-          <t>47,238</t>
+          <t>47,408</t>
         </is>
       </c>
       <c r="M850" t="n">
@@ -56634,7 +56634,7 @@
       </c>
       <c r="L852" t="inlineStr">
         <is>
-          <t>509,542</t>
+          <t>512,535</t>
         </is>
       </c>
       <c r="M852" t="n">
@@ -56766,7 +56766,7 @@
       </c>
       <c r="L854" t="inlineStr">
         <is>
-          <t>277,661</t>
+          <t>279,074</t>
         </is>
       </c>
       <c r="M854" t="n">
@@ -57360,7 +57360,7 @@
       </c>
       <c r="L863" t="inlineStr">
         <is>
-          <t>730,384</t>
+          <t>732,746</t>
         </is>
       </c>
       <c r="M863" t="n">
@@ -57888,7 +57888,7 @@
       </c>
       <c r="L871" t="inlineStr">
         <is>
-          <t>53,059</t>
+          <t>53,207</t>
         </is>
       </c>
       <c r="M871" t="n">
@@ -58020,7 +58020,7 @@
       </c>
       <c r="L873" t="inlineStr">
         <is>
-          <t>59,877</t>
+          <t>60,201</t>
         </is>
       </c>
       <c r="M873" t="n">
@@ -58482,7 +58482,7 @@
       </c>
       <c r="L880" t="inlineStr">
         <is>
-          <t>144,620</t>
+          <t>145,044</t>
         </is>
       </c>
       <c r="M880" t="n">
@@ -59406,7 +59406,7 @@
       </c>
       <c r="L894" t="inlineStr">
         <is>
-          <t>41,129</t>
+          <t>41,301</t>
         </is>
       </c>
       <c r="M894" t="n">
@@ -60264,7 +60264,7 @@
       </c>
       <c r="L907" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>187</t>
         </is>
       </c>
       <c r="M907" t="inlineStr"/>
@@ -61780,7 +61780,7 @@
       </c>
       <c r="L930" t="inlineStr">
         <is>
-          <t>47,005</t>
+          <t>47,180</t>
         </is>
       </c>
       <c r="M930" t="n">
@@ -61912,7 +61912,7 @@
       </c>
       <c r="L932" t="inlineStr">
         <is>
-          <t>36,187</t>
+          <t>36,358</t>
         </is>
       </c>
       <c r="M932" t="n">
@@ -62374,7 +62374,7 @@
       </c>
       <c r="L939" t="inlineStr">
         <is>
-          <t>180,598</t>
+          <t>180,998</t>
         </is>
       </c>
       <c r="M939" t="n">
@@ -63034,7 +63034,7 @@
       </c>
       <c r="L949" t="inlineStr">
         <is>
-          <t>407,672</t>
+          <t>408,829</t>
         </is>
       </c>
       <c r="M949" t="n">
@@ -64222,7 +64222,7 @@
       </c>
       <c r="L967" t="inlineStr">
         <is>
-          <t>175,269</t>
+          <t>175,961</t>
         </is>
       </c>
       <c r="M967" t="n">

</xml_diff>